<commit_message>
Changes in the excel file
</commit_message>
<xml_diff>
--- a/DataBaseDesign.xlsx
+++ b/DataBaseDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jap Purohit\eclipse-workspace\ECollegeProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C569F80F-AD08-476D-A7E2-08F42F39A9EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510DE692-7D4D-4BA1-B706-609D2AE571D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4776" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="107">
   <si>
     <t>first_name</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t>securityAnswer</t>
+  </si>
+  <si>
+    <t>image_path</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -500,6 +503,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -527,8 +532,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,48 +875,48 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="E2" s="17" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="E2" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
-      <c r="I2" s="17" t="s">
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="I2" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="19"/>
-      <c r="M2" s="17" t="s">
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
+      <c r="M2" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="18"/>
-      <c r="O2" s="19"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="21"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
+      <c r="A3" s="16"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="E3" s="14"/>
+      <c r="E3" s="16"/>
       <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="13"/>
+      <c r="M3" s="15"/>
       <c r="N3" s="1" t="s">
         <v>24</v>
       </c>
@@ -920,22 +925,22 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="15"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="15"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="I4" s="13"/>
+      <c r="I4" s="15"/>
       <c r="J4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="M4" s="13"/>
+      <c r="M4" s="15"/>
       <c r="N4" s="1" t="s">
         <v>20</v>
       </c>
@@ -944,24 +949,24 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="15"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="I5" s="13"/>
+      <c r="I5" s="15"/>
       <c r="J5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="M5" s="13"/>
+      <c r="M5" s="15"/>
       <c r="N5" s="1" t="s">
         <v>14</v>
       </c>
@@ -970,22 +975,22 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="E6" s="15"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="I6" s="13"/>
+      <c r="I6" s="15"/>
       <c r="J6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="M6" s="13"/>
+      <c r="M6" s="15"/>
       <c r="N6" s="1" t="s">
         <v>25</v>
       </c>
@@ -994,22 +999,22 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="E7" s="15"/>
+      <c r="E7" s="17"/>
       <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="I7" s="13"/>
+      <c r="I7" s="15"/>
       <c r="J7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="M7" s="13"/>
+      <c r="M7" s="15"/>
       <c r="N7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1018,170 +1023,170 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="15"/>
+      <c r="E8" s="17"/>
       <c r="F8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="I8" s="13"/>
+      <c r="I8" s="15"/>
       <c r="J8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="M8" s="13"/>
+      <c r="M8" s="15"/>
       <c r="N8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="15"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="13"/>
+      <c r="I9" s="15"/>
       <c r="J9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="M9" s="13"/>
+      <c r="M9" s="15"/>
       <c r="N9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="3" t="s">
         <v>47</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="I10" s="13"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="M10" s="13"/>
+      <c r="M10" s="15"/>
       <c r="N10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="I11" s="13"/>
+      <c r="I11" s="15"/>
       <c r="J11" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="M11" s="13"/>
+      <c r="M11" s="15"/>
       <c r="N11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="I12" s="13"/>
+      <c r="I12" s="15"/>
       <c r="J12" s="3" t="s">
         <v>53</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="M12" s="13"/>
+      <c r="M12" s="15"/>
       <c r="N12" s="3" t="s">
         <v>38</v>
       </c>
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="M13" s="13"/>
+      <c r="M13" s="15"/>
       <c r="N13" s="3" t="s">
         <v>48</v>
       </c>
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="M14" s="13"/>
+      <c r="M14" s="15"/>
       <c r="N14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="13"/>
+      <c r="M15" s="15"/>
       <c r="N15" s="3" t="s">
         <v>50</v>
       </c>
       <c r="O15" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="21"/>
-      <c r="E17" s="17" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="E17" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="19"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="14"/>
+      <c r="E18" s="16"/>
       <c r="F18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1190,12 +1195,12 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="15"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="1" t="s">
         <v>33</v>
       </c>
@@ -1204,28 +1209,28 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E20" s="15"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E21" s="15"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="15"/>
+      <c r="E22" s="17"/>
       <c r="F22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E23" s="16"/>
+      <c r="E23" s="18"/>
       <c r="F23" s="3" t="s">
         <v>51</v>
       </c>
@@ -1252,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:J58"/>
+  <dimension ref="B1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="B7:D22"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1472,7 +1477,7 @@
       <c r="D21" t="s">
         <v>93</v>
       </c>
-      <c r="H21" s="22"/>
+      <c r="H21" s="13"/>
       <c r="I21" s="9"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
@@ -1486,7 +1491,7 @@
       <c r="I22" s="9"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="23"/>
+      <c r="B23" s="14"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
     </row>
@@ -1661,124 +1666,125 @@
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" t="s">
+        <v>93</v>
+      </c>
       <c r="H38">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="25"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="6" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="C41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D41" t="s">
         <v>93</v>
-      </c>
-      <c r="I41" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D42" t="s">
         <v>93</v>
       </c>
-      <c r="H42">
-        <v>1</v>
-      </c>
       <c r="I42" t="s">
-        <v>91</v>
-      </c>
-      <c r="J42" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>16</v>
+        <v>76</v>
+      </c>
+      <c r="C43" t="s">
+        <v>100</v>
       </c>
       <c r="D43" t="s">
         <v>93</v>
       </c>
       <c r="H43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>89</v>
-      </c>
-      <c r="J43">
-        <v>0</v>
+        <v>91</v>
+      </c>
+      <c r="J43" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" t="s">
+        <v>93</v>
+      </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44" t="s">
+        <v>89</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
         <v>68</v>
       </c>
-      <c r="D44" t="s">
-        <v>93</v>
-      </c>
-      <c r="H44">
+      <c r="D45" t="s">
+        <v>93</v>
+      </c>
+      <c r="H45">
         <v>3</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I45" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="H45">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H46">
         <v>4</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I46" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B46" s="6" t="s">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B47" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="H46">
+      <c r="H47">
         <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
-        <v>79</v>
-      </c>
-      <c r="C47" t="s">
-        <v>97</v>
-      </c>
-      <c r="D47" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="C48" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D48" t="s">
         <v>93</v>
@@ -1786,10 +1792,10 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D49" t="s">
         <v>93</v>
@@ -1797,34 +1803,34 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
         <v>80</v>
       </c>
-      <c r="D50" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B52" s="6" t="s">
+      <c r="D51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B53" s="6" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" t="s">
-        <v>102</v>
-      </c>
-      <c r="D53" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="C54" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D54" t="s">
         <v>93</v>
@@ -1832,7 +1838,10 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>16</v>
+        <v>76</v>
+      </c>
+      <c r="C55" t="s">
+        <v>100</v>
       </c>
       <c r="D55" t="s">
         <v>93</v>
@@ -1840,7 +1849,7 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="D56" t="s">
         <v>93</v>
@@ -1848,7 +1857,7 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="D57" t="s">
         <v>93</v>
@@ -1856,12 +1865,20 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
+        <v>81</v>
+      </c>
+      <c r="D58" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
         <v>25</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>99</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Database Creation Query Started
</commit_message>
<xml_diff>
--- a/DataBaseDesign.xlsx
+++ b/DataBaseDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jap Purohit\eclipse-workspace\ECollegeProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2137C5C7-DDC8-45CE-8E06-8A0D7F854986}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE35717-8123-40B9-BDB5-5F6F01ABED64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="1872" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="138">
   <si>
     <t>first_name</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>subcategory_name</t>
+  </si>
+  <si>
+    <t>Trigger Creation Left</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -580,7 +583,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -951,48 +953,48 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="E2" s="16" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="E2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
-      <c r="I2" s="16" t="s">
+      <c r="F2" s="18"/>
+      <c r="G2" s="19"/>
+      <c r="I2" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
-      <c r="M2" s="16" t="s">
+      <c r="J2" s="16"/>
+      <c r="K2" s="17"/>
+      <c r="M2" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="17"/>
-      <c r="O2" s="18"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="17"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="E3" s="13"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="12"/>
+      <c r="I3" s="11"/>
       <c r="J3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="12"/>
+      <c r="M3" s="11"/>
       <c r="N3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1001,22 +1003,22 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="14"/>
+      <c r="E4" s="13"/>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="I4" s="12"/>
+      <c r="I4" s="11"/>
       <c r="J4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="M4" s="12"/>
+      <c r="M4" s="11"/>
       <c r="N4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1025,24 +1027,24 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="14"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="I5" s="12"/>
+      <c r="I5" s="11"/>
       <c r="J5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="M5" s="12"/>
+      <c r="M5" s="11"/>
       <c r="N5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1051,22 +1053,22 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="E6" s="14"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="I6" s="12"/>
+      <c r="I6" s="11"/>
       <c r="J6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="M6" s="12"/>
+      <c r="M6" s="11"/>
       <c r="N6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1075,22 +1077,22 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="E7" s="14"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="I7" s="12"/>
+      <c r="I7" s="11"/>
       <c r="J7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="M7" s="12"/>
+      <c r="M7" s="11"/>
       <c r="N7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1099,170 +1101,170 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="I8" s="12"/>
+      <c r="I8" s="11"/>
       <c r="J8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="M8" s="12"/>
+      <c r="M8" s="11"/>
       <c r="N8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="14"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="12"/>
+      <c r="I9" s="11"/>
       <c r="J9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="M9" s="12"/>
+      <c r="M9" s="11"/>
       <c r="N9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="E10" s="15"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="3" t="s">
         <v>47</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="I10" s="12"/>
+      <c r="I10" s="11"/>
       <c r="J10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="M10" s="12"/>
+      <c r="M10" s="11"/>
       <c r="N10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="I11" s="12"/>
+      <c r="I11" s="11"/>
       <c r="J11" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="M11" s="12"/>
+      <c r="M11" s="11"/>
       <c r="N11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="I12" s="12"/>
+      <c r="I12" s="11"/>
       <c r="J12" s="3" t="s">
         <v>53</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="M12" s="12"/>
+      <c r="M12" s="11"/>
       <c r="N12" s="3" t="s">
         <v>38</v>
       </c>
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="M13" s="12"/>
+      <c r="M13" s="11"/>
       <c r="N13" s="3" t="s">
         <v>48</v>
       </c>
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="M14" s="12"/>
+      <c r="M14" s="11"/>
       <c r="N14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="12"/>
+      <c r="M15" s="11"/>
       <c r="N15" s="3" t="s">
         <v>50</v>
       </c>
       <c r="O15" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-      <c r="E17" s="16" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="E17" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="13"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1271,12 +1273,12 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="14"/>
+      <c r="E19" s="13"/>
       <c r="F19" s="1" t="s">
         <v>33</v>
       </c>
@@ -1285,28 +1287,28 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E20" s="14"/>
+      <c r="E20" s="13"/>
       <c r="F20" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E21" s="14"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="14"/>
+      <c r="E22" s="13"/>
       <c r="F22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E23" s="15"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="3" t="s">
         <v>51</v>
       </c>
@@ -1335,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1642,7 +1644,9 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="9"/>
+      <c r="B23" s="7" t="s">
+        <v>137</v>
+      </c>
       <c r="E23">
         <v>5</v>
       </c>
@@ -1796,7 +1800,7 @@
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>105</v>
       </c>
       <c r="C38" t="s">
@@ -1807,7 +1811,7 @@
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="11"/>
+      <c r="B39" s="10"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" s="6" t="s">

</xml_diff>

<commit_message>
Changes in query file
</commit_message>
<xml_diff>
--- a/DataBaseDesign.xlsx
+++ b/DataBaseDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jap Purohit\eclipse-workspace\ECollegeProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE35717-8123-40B9-BDB5-5F6F01ABED64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF406BE3-4EE7-49B2-9FE0-63A8A2724719}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1872" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="204" yWindow="2892" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="139">
   <si>
     <t>first_name</t>
   </si>
@@ -440,7 +440,10 @@
     <t>subcategory_name</t>
   </si>
   <si>
-    <t>Trigger Creation Left</t>
+    <t>productDescirption</t>
+  </si>
+  <si>
+    <t>sub_category_id</t>
   </si>
 </sst>
 </file>
@@ -1335,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:G64"/>
+  <dimension ref="B1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1644,9 +1647,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="B23" s="7"/>
       <c r="E23">
         <v>5</v>
       </c>
@@ -1697,6 +1698,9 @@
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>135</v>
       </c>
@@ -1811,41 +1815,29 @@
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="10"/>
+      <c r="B39" s="9" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="10"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="6" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" t="s">
-        <v>96</v>
-      </c>
-      <c r="D41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" t="s">
-        <v>98</v>
-      </c>
-      <c r="D42" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D43" t="s">
         <v>92</v>
@@ -1853,7 +1845,10 @@
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="C44" t="s">
+        <v>98</v>
       </c>
       <c r="D44" t="s">
         <v>92</v>
@@ -1861,45 +1856,42 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
         <v>68</v>
       </c>
-      <c r="D45" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="6" t="s">
+      <c r="D47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="6" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>79</v>
-      </c>
-      <c r="C48" t="s">
-        <v>96</v>
-      </c>
-      <c r="D48" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
-        <v>25</v>
-      </c>
-      <c r="C49" t="s">
-        <v>98</v>
-      </c>
-      <c r="D49" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="C50" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D50" t="s">
         <v>92</v>
@@ -1907,7 +1899,10 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>80</v>
+        <v>25</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
       </c>
       <c r="D51" t="s">
         <v>92</v>
@@ -1915,7 +1910,10 @@
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>113</v>
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>100</v>
       </c>
       <c r="D52" t="s">
         <v>92</v>
@@ -1923,7 +1921,7 @@
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="D53" t="s">
         <v>92</v>
@@ -1931,7 +1929,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D54" t="s">
         <v>92</v>
@@ -1939,7 +1937,7 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D55" t="s">
         <v>92</v>
@@ -1947,42 +1945,39 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>116</v>
+      </c>
+      <c r="D57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
         <v>117</v>
       </c>
-      <c r="D56" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B58" s="6" t="s">
+      <c r="D58" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B60" s="6" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B59" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" t="s">
-        <v>101</v>
-      </c>
-      <c r="D59" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B60" t="s">
-        <v>76</v>
-      </c>
-      <c r="C60" t="s">
-        <v>99</v>
-      </c>
-      <c r="D60" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="C61" t="s">
+        <v>101</v>
       </c>
       <c r="D61" t="s">
         <v>92</v>
@@ -1990,7 +1985,10 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>68</v>
+        <v>76</v>
+      </c>
+      <c r="C62" t="s">
+        <v>99</v>
       </c>
       <c r="D62" t="s">
         <v>92</v>
@@ -1998,7 +1996,7 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="D63" t="s">
         <v>92</v>
@@ -2006,12 +2004,28 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
+        <v>68</v>
+      </c>
+      <c r="D64" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>81</v>
+      </c>
+      <c r="D65" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
         <v>25</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C66" t="s">
         <v>98</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D66" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Admin Panel, Product Details, Add Users and Validation for users done
</commit_message>
<xml_diff>
--- a/DataBaseDesign.xlsx
+++ b/DataBaseDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jap Purohit\eclipse-workspace\ECollegeProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF406BE3-4EE7-49B2-9FE0-63A8A2724719}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8385D9C-D9DF-4847-8B98-24E76D363E02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="204" yWindow="2892" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1340,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Bean and Dao Creation done and Admin Panel Designing Done
</commit_message>
<xml_diff>
--- a/DataBaseDesign.xlsx
+++ b/DataBaseDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jap Purohit\eclipse-workspace\ECollegeProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8385D9C-D9DF-4847-8B98-24E76D363E02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C57B80B-7786-4FA7-9FB6-CF95DDD255D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="204" yWindow="2892" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,12 +467,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -576,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -615,6 +621,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1340,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1968,64 +1976,69 @@
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="20" t="s">
         <v>78</v>
       </c>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B61" t="s">
+      <c r="B61" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B62" t="s">
+      <c r="B62" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B63" t="s">
+      <c r="B63" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D63" t="s">
+      <c r="C63" s="21"/>
+      <c r="D63" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B64" t="s">
+      <c r="B64" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D64" t="s">
+      <c r="C64" s="21"/>
+      <c r="D64" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B65" t="s">
+      <c r="B65" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D65" t="s">
+      <c r="C65" s="21"/>
+      <c r="D65" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B66" t="s">
+      <c r="B66" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="21" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"Two Trigger integrated with front-end and working superbly fine" 1- Email Validation Trigger Done 2- Password Change Trigger Done Front-end improved and made more dynamic. Code Pushed
</commit_message>
<xml_diff>
--- a/DataBaseDesign.xlsx
+++ b/DataBaseDesign.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jap Purohit\eclipse-workspace\ECollegeProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C57B80B-7786-4FA7-9FB6-CF95DDD255D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF92CF8-F62B-453C-A2AA-84063B32B325}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="204" yWindow="2892" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1404" yWindow="1404" windowWidth="15336" windowHeight="8136" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="145">
   <si>
     <t>first_name</t>
   </si>
@@ -444,6 +444,24 @@
   </si>
   <si>
     <t>sub_category_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cart </t>
+  </si>
+  <si>
+    <t>productid</t>
+  </si>
+  <si>
+    <t>checkout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">order </t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>orderdetail</t>
   </si>
 </sst>
 </file>
@@ -582,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -594,6 +612,8 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -621,8 +641,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -964,48 +985,48 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
-      <c r="E2" s="15" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="E2" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-      <c r="I2" s="15" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="I2" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="17"/>
-      <c r="M2" s="15" t="s">
+      <c r="J2" s="18"/>
+      <c r="K2" s="19"/>
+      <c r="M2" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="16"/>
-      <c r="O2" s="17"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="19"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="E3" s="12"/>
+      <c r="E3" s="14"/>
       <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="11"/>
+      <c r="I3" s="13"/>
       <c r="J3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="11"/>
+      <c r="M3" s="13"/>
       <c r="N3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1014,22 +1035,22 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="13"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="I4" s="11"/>
+      <c r="I4" s="13"/>
       <c r="J4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="M4" s="11"/>
+      <c r="M4" s="13"/>
       <c r="N4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1038,24 +1059,24 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="15"/>
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="I5" s="11"/>
+      <c r="I5" s="13"/>
       <c r="J5" s="5" t="s">
         <v>23</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="M5" s="11"/>
+      <c r="M5" s="13"/>
       <c r="N5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1064,22 +1085,22 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="E6" s="13"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="I6" s="11"/>
+      <c r="I6" s="13"/>
       <c r="J6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="M6" s="11"/>
+      <c r="M6" s="13"/>
       <c r="N6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1088,22 +1109,22 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="E7" s="13"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="I7" s="11"/>
+      <c r="I7" s="13"/>
       <c r="J7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="M7" s="11"/>
+      <c r="M7" s="13"/>
       <c r="N7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1112,170 +1133,170 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="I8" s="11"/>
+      <c r="I8" s="13"/>
       <c r="J8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="M8" s="11"/>
+      <c r="M8" s="13"/>
       <c r="N8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="13"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="13"/>
       <c r="J9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="M9" s="11"/>
+      <c r="M9" s="13"/>
       <c r="N9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="3" t="s">
         <v>47</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="I10" s="11"/>
+      <c r="I10" s="13"/>
       <c r="J10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="M10" s="11"/>
+      <c r="M10" s="13"/>
       <c r="N10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="I11" s="11"/>
+      <c r="I11" s="13"/>
       <c r="J11" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="M11" s="11"/>
+      <c r="M11" s="13"/>
       <c r="N11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="I12" s="11"/>
+      <c r="I12" s="13"/>
       <c r="J12" s="3" t="s">
         <v>53</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="M12" s="11"/>
+      <c r="M12" s="13"/>
       <c r="N12" s="3" t="s">
         <v>38</v>
       </c>
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="M13" s="11"/>
+      <c r="M13" s="13"/>
       <c r="N13" s="3" t="s">
         <v>48</v>
       </c>
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="M14" s="11"/>
+      <c r="M14" s="13"/>
       <c r="N14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="11"/>
+      <c r="M15" s="13"/>
       <c r="N15" s="3" t="s">
         <v>50</v>
       </c>
       <c r="O15" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="E17" s="15" t="s">
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="E17" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="17"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="12"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1284,12 +1305,12 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="E19" s="13"/>
+      <c r="E19" s="15"/>
       <c r="F19" s="1" t="s">
         <v>33</v>
       </c>
@@ -1298,28 +1319,28 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E20" s="13"/>
+      <c r="E20" s="15"/>
       <c r="F20" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E21" s="13"/>
+      <c r="E21" s="15"/>
       <c r="F21" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="13"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E23" s="14"/>
+      <c r="E23" s="16"/>
       <c r="F23" s="3" t="s">
         <v>51</v>
       </c>
@@ -1346,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:G66"/>
+  <dimension ref="B1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1596,7 +1617,7 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="12" t="s">
         <v>91</v>
       </c>
       <c r="G19" t="s">
@@ -1630,7 +1651,7 @@
       <c r="E21">
         <v>3</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="12" t="s">
         <v>90</v>
       </c>
       <c r="G21" t="s">
@@ -1659,7 +1680,7 @@
       <c r="E23">
         <v>5</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="12" t="s">
         <v>110</v>
       </c>
       <c r="G23" t="s">
@@ -1889,12 +1910,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>79</v>
       </c>
@@ -1905,7 +1926,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>25</v>
       </c>
@@ -1916,7 +1937,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>4</v>
       </c>
@@ -1927,7 +1948,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>80</v>
       </c>
@@ -1935,7 +1956,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>113</v>
       </c>
@@ -1943,7 +1964,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>112</v>
       </c>
@@ -1951,7 +1972,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>114</v>
       </c>
@@ -1959,87 +1980,160 @@
         <v>92</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>116</v>
       </c>
       <c r="D57" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F57" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>117</v>
       </c>
       <c r="D58" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B60" s="20" t="s">
+      <c r="F58" t="s">
+        <v>140</v>
+      </c>
+      <c r="G58" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B60" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B61" s="21" t="s">
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="G60" s="22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B61" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="21" t="s">
+      <c r="C61" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D61" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B62" s="21" t="s">
+      <c r="D61" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F61">
+        <v>3</v>
+      </c>
+      <c r="G61" s="22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B62" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C62" s="21" t="s">
+      <c r="C62" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D62" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B63" s="21" t="s">
+      <c r="D62" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B63" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="21"/>
-      <c r="D63" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B64" s="21" t="s">
+      <c r="C63" s="12"/>
+      <c r="D63" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F63" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B64" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="21"/>
-      <c r="D64" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B65" s="21" t="s">
+      <c r="C64" s="12"/>
+      <c r="D64" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B65" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C65" s="21"/>
-      <c r="D65" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B66" s="21" t="s">
+      <c r="C65" s="12"/>
+      <c r="D65" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B66" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C66" s="21" t="s">
+      <c r="C66" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D66" s="21" t="s">
-        <v>92</v>
+      <c r="D66" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F67" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E69" t="s">
+        <v>143</v>
+      </c>
+      <c r="F69">
+        <v>1</v>
+      </c>
+      <c r="G69">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F71" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F75">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>